<commit_message>
Add print permit to excel.
</commit_message>
<xml_diff>
--- a/template/permit_template.xlsx
+++ b/template/permit_template.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Наряд\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\Permit\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Бланк" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,9 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>на производство работ на высоте</t>
+  </si>
+  <si>
+    <t>Выдан  #date_write#</t>
+  </si>
+  <si>
+    <t>Действителен до   #date_limit#</t>
+  </si>
+  <si>
+    <t>1. Ответственный руководителю работ</t>
+  </si>
+  <si>
+    <t>(Ф.И.О., должность)</t>
+  </si>
+  <si>
+    <t>#initials_supervisor#, #post_supervisor#</t>
   </si>
   <si>
     <r>
@@ -36,7 +51,7 @@
       <rPr>
         <b/>
         <u/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -47,17 +62,153 @@
     </r>
   </si>
   <si>
-    <t>Выдан  #date_write#</t>
-  </si>
-  <si>
-    <t>Действителен до   #date_write#</t>
+    <t>2. Ответственный исполнитель работ</t>
+  </si>
+  <si>
+    <t>#initials_executor#, #post_executor#</t>
+  </si>
+  <si>
+    <t>3. На выполнение работ</t>
+  </si>
+  <si>
+    <t>(наименование работ, место)</t>
+  </si>
+  <si>
+    <t>#permit_name#, #permit_place#</t>
+  </si>
+  <si>
+    <t>Фамилия, имя, отчество</t>
+  </si>
+  <si>
+    <t>С условиями работ ознакомил целевой инструктаж провел</t>
+  </si>
+  <si>
+    <t>С условиями работ ознакомлен, целевой инструктаж получил</t>
+  </si>
+  <si>
+    <t>5. Место выполнения работ</t>
+  </si>
+  <si>
+    <t>(место)</t>
+  </si>
+  <si>
+    <t>#permit_place#</t>
+  </si>
+  <si>
+    <t>#content_work#</t>
+  </si>
+  <si>
+    <t>#start_work#</t>
+  </si>
+  <si>
+    <t>#end_work#</t>
+  </si>
+  <si>
+    <t>Содержание работ:</t>
+  </si>
+  <si>
+    <t>Условия проведения работ:</t>
+  </si>
+  <si>
+    <t>#condition_work#</t>
+  </si>
+  <si>
+    <t>Начало работ:</t>
+  </si>
+  <si>
+    <t>Окончание работ:</t>
+  </si>
+  <si>
+    <t>4. Состав исполнителей работ: #executors#</t>
+  </si>
+  <si>
+    <t>Системы обеспечения безопасности работ на высоте</t>
+  </si>
+  <si>
+    <t>Состав системы</t>
+  </si>
+  <si>
+    <t>Удерживающие системы</t>
+  </si>
+  <si>
+    <t>Системы позиционирования</t>
+  </si>
+  <si>
+    <t>Страховочные системы</t>
+  </si>
+  <si>
+    <t>Эвакуационные и спасательные системы</t>
+  </si>
+  <si>
+    <t>6. Системы обеспечения безопасности работ на высоте:</t>
+  </si>
+  <si>
+    <t>#retaining_system#</t>
+  </si>
+  <si>
+    <t>#position_system#</t>
+  </si>
+  <si>
+    <t>#safety_system#</t>
+  </si>
+  <si>
+    <t>#rescue_system#</t>
+  </si>
+  <si>
+    <t>Необходимые для производства работ:</t>
+  </si>
+  <si>
+    <t>Материалы:</t>
+  </si>
+  <si>
+    <t>Инструменты:</t>
+  </si>
+  <si>
+    <t>Приспособления:</t>
+  </si>
+  <si>
+    <t>#materials#</t>
+  </si>
+  <si>
+    <t>#instruments#</t>
+  </si>
+  <si>
+    <t>#adaptations#</t>
+  </si>
+  <si>
+    <t>№
+п/п</t>
+  </si>
+  <si>
+    <t>Наименование мероприятий или ссылка на пункт ППР или технологических карт</t>
+  </si>
+  <si>
+    <t>Срок выполнения</t>
+  </si>
+  <si>
+    <t>Ответственные исполнители</t>
+  </si>
+  <si>
+    <t>7. До начала производства работ необходимо выполнить следующие мероприятия: #begin_event#</t>
+  </si>
+  <si>
+    <t>8. В процессе производства работ необходимо выполнить следующие мероприятия: #proc_event#</t>
+  </si>
+  <si>
+    <t>9. Особые услови проведения работ: #special_event#</t>
+  </si>
+  <si>
+    <t>Наименование мероприятий</t>
+  </si>
+  <si>
+    <t>Наименование условия</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,8 +218,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,7 +254,7 @@
     <font>
       <b/>
       <u/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -94,7 +270,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -102,16 +278,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -394,56 +805,741 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G8"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="41"/>
+      <c r="C13" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="41"/>
+      <c r="C16" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="45"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="41"/>
+      <c r="C23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="43"/>
+      <c r="C26" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="39"/>
+      <c r="C31" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="38"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="24"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="24"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="24"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="32"/>
+      <c r="C44" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="32"/>
+      <c r="C46" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="31"/>
+      <c r="C48" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+    </row>
+    <row r="51" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" s="30"/>
+      <c r="H51" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I51" s="28"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="11"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+    </row>
+    <row r="55" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" s="30"/>
+      <c r="H55" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I55" s="28"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="11"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+    </row>
+    <row r="59" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G59" s="30"/>
+      <c r="H59" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I59" s="28"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="45">
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="A58:I58"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="A13:B14"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A50:I50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A48:B48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add writer to permit template.
</commit_message>
<xml_diff>
--- a/template/permit_template.xlsx
+++ b/template/permit_template.xlsx
@@ -38,24 +38,6 @@
     <t>(Ф.И.О., должность)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Наряд-допуск № </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>#serial_number#</t>
-    </r>
-  </si>
-  <si>
     <t>2. Ответственный исполнитель работ</t>
   </si>
   <si>
@@ -344,6 +326,24 @@
   </si>
   <si>
     <t>(наименование работ)</t>
+  </si>
+  <si>
+    <r>
+      <t>Наряд-допуск № «</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#serial_number#»</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -652,26 +652,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -682,68 +664,11 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -768,11 +693,86 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48:I48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,27 +1101,27 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="B4" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
@@ -1139,12 +1139,12 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1152,12 +1152,12 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="C8" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1174,32 +1174,32 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="48" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1213,32 +1213,32 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="A13" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="48" t="s">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1252,32 +1252,32 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
+      <c r="A16" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="67"/>
+      <c r="C16" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
-      <c r="C17" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -1304,21 +1304,21 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="55" t="s">
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="56"/>
-      <c r="I20" s="57"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="70"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
@@ -1332,32 +1332,32 @@
       <c r="I21" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
+      <c r="A23" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="67"/>
+      <c r="C23" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
-      <c r="C24" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
+      <c r="C24" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
@@ -1371,19 +1371,19 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
+      <c r="A26" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="57"/>
+      <c r="C26" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
@@ -1397,19 +1397,19 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="58"/>
+      <c r="C28" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
@@ -1435,18 +1435,18 @@
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="62"/>
-      <c r="C31" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
+      <c r="C31" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
@@ -1461,18 +1461,18 @@
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="62"/>
-      <c r="C33" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
+      <c r="C33" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
@@ -1486,13 +1486,13 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
+      <c r="A35" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -1500,78 +1500,78 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="35"/>
       <c r="C36" s="35"/>
       <c r="D36" s="35"/>
       <c r="E36" s="36"/>
       <c r="F36" s="59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G36" s="60"/>
       <c r="H36" s="60"/>
       <c r="I36" s="61"/>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="76"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="77"/>
+    </row>
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="42" t="s">
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="44"/>
-    </row>
-    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="77"/>
+    </row>
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="42" t="s">
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="44"/>
-    </row>
-    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="77"/>
+    </row>
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="42" t="s">
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="44"/>
-    </row>
-    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="76"/>
+      <c r="I40" s="77"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
@@ -1585,12 +1585,12 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
+      <c r="A42" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -1609,19 +1609,19 @@
       <c r="I43" s="11"/>
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
+      <c r="A44" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="72"/>
+      <c r="C44" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
@@ -1635,19 +1635,19 @@
       <c r="I45" s="11"/>
     </row>
     <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
+      <c r="A46" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="73"/>
+      <c r="C46" s="74" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="74"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
@@ -1661,19 +1661,19 @@
       <c r="I47" s="11"/>
     </row>
     <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
+      <c r="A48" s="72" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="72"/>
+      <c r="C48" s="74" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="74"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
@@ -1701,28 +1701,28 @@
     </row>
     <row r="51" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="34" t="s">
         <v>40</v>
-      </c>
-      <c r="B51" s="34" t="s">
-        <v>41</v>
       </c>
       <c r="C51" s="35"/>
       <c r="D51" s="35"/>
       <c r="E51" s="36"/>
       <c r="F51" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G51" s="38"/>
       <c r="H51" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I51" s="36"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="15"/>
-      <c r="C52" s="77"/>
-      <c r="D52" s="77"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
       <c r="E52" s="16"/>
       <c r="F52" s="15"/>
       <c r="G52" s="18"/>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54" s="33"/>
       <c r="C54" s="33"/>
@@ -1744,28 +1744,28 @@
     </row>
     <row r="55" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C55" s="35"/>
       <c r="D55" s="35"/>
       <c r="E55" s="36"/>
       <c r="F55" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G55" s="38"/>
       <c r="H55" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I55" s="36"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="31"/>
       <c r="B56" s="15"/>
-      <c r="C56" s="77"/>
-      <c r="D56" s="77"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
       <c r="E56" s="16"/>
       <c r="F56" s="15"/>
       <c r="G56" s="18"/>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B58" s="33"/>
       <c r="C58" s="33"/>
@@ -1787,28 +1787,28 @@
     </row>
     <row r="59" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B59" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C59" s="35"/>
       <c r="D59" s="35"/>
       <c r="E59" s="36"/>
       <c r="F59" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G59" s="38"/>
       <c r="H59" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I59" s="36"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="31"/>
       <c r="B60" s="15"/>
-      <c r="C60" s="77"/>
-      <c r="D60" s="77"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
       <c r="E60" s="16"/>
       <c r="F60" s="15"/>
       <c r="G60" s="18"/>
@@ -1816,13 +1816,13 @@
       <c r="I60" s="16"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="76" t="s">
-        <v>49</v>
-      </c>
-      <c r="B62" s="76"/>
-      <c r="C62" s="76"/>
-      <c r="D62" s="76"/>
-      <c r="E62" s="76"/>
+      <c r="A62" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
       <c r="F62" s="33"/>
       <c r="G62" s="33"/>
       <c r="H62" s="33"/>
@@ -1830,31 +1830,31 @@
     </row>
     <row r="63" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="35"/>
       <c r="D63" s="35"/>
       <c r="E63" s="36"/>
       <c r="F63" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G63" s="18"/>
       <c r="H63" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I63" s="16"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="71"/>
-      <c r="B64" s="72"/>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="73"/>
-      <c r="F64" s="71"/>
-      <c r="G64" s="73"/>
-      <c r="H64" s="74"/>
-      <c r="I64" s="75"/>
+      <c r="A64" s="46"/>
+      <c r="B64" s="47"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="50"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
@@ -1868,25 +1868,25 @@
       <c r="I65" s="10"/>
     </row>
     <row r="66" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="46" t="s">
+      <c r="A66" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66" s="40"/>
+      <c r="C66" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D66" s="41"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="41"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
+    </row>
+    <row r="67" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="40"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="52" t="s">
         <v>53</v>
-      </c>
-      <c r="B66" s="46"/>
-      <c r="C66" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="47"/>
-      <c r="H66" s="47"/>
-      <c r="I66" s="47"/>
-    </row>
-    <row r="67" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="46"/>
-      <c r="B67" s="46"/>
-      <c r="C67" s="52" t="s">
-        <v>54</v>
       </c>
       <c r="D67" s="52"/>
       <c r="E67" s="52"/>
@@ -1907,32 +1907,32 @@
       <c r="I68" s="10"/>
     </row>
     <row r="69" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B69" s="46"/>
-      <c r="C69" s="47" t="s">
+      <c r="A69" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" s="40"/>
+      <c r="C69" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
+      <c r="G69" s="41"/>
+      <c r="H69" s="41"/>
+      <c r="I69" s="41"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="40"/>
+      <c r="B70" s="40"/>
+      <c r="C70" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="47"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="46"/>
-      <c r="B70" s="46"/>
-      <c r="C70" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="48"/>
-      <c r="I70" s="48"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
+      <c r="H70" s="42"/>
+      <c r="I70" s="42"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
@@ -1946,32 +1946,32 @@
       <c r="I71" s="10"/>
     </row>
     <row r="72" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" s="46"/>
-      <c r="C72" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
-      <c r="F72" s="47"/>
-      <c r="G72" s="47"/>
-      <c r="H72" s="47"/>
-      <c r="I72" s="47"/>
+      <c r="A72" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B72" s="40"/>
+      <c r="C72" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="41"/>
+      <c r="I72" s="41"/>
     </row>
     <row r="73" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="46"/>
-      <c r="B73" s="46"/>
-      <c r="C73" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="D73" s="69"/>
-      <c r="E73" s="69"/>
-      <c r="F73" s="69"/>
-      <c r="G73" s="69"/>
-      <c r="H73" s="69"/>
-      <c r="I73" s="69"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="43"/>
+      <c r="I73" s="43"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
@@ -1985,32 +1985,32 @@
       <c r="I74" s="10"/>
     </row>
     <row r="75" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="B75" s="46"/>
-      <c r="C75" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="47"/>
-      <c r="H75" s="47"/>
-      <c r="I75" s="47"/>
+      <c r="A75" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" s="40"/>
+      <c r="C75" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D75" s="41"/>
+      <c r="E75" s="41"/>
+      <c r="F75" s="41"/>
+      <c r="G75" s="41"/>
+      <c r="H75" s="41"/>
+      <c r="I75" s="41"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="46"/>
-      <c r="B76" s="46"/>
-      <c r="C76" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="48"/>
-      <c r="G76" s="48"/>
-      <c r="H76" s="48"/>
-      <c r="I76" s="48"/>
+      <c r="A76" s="40"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="42"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
@@ -2024,28 +2024,28 @@
       <c r="I77" s="10"/>
     </row>
     <row r="78" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="B78" s="53"/>
-      <c r="C78" s="53"/>
-      <c r="D78" s="53"/>
-      <c r="E78" s="53"/>
-      <c r="F78" s="53"/>
-      <c r="G78" s="53"/>
-      <c r="H78" s="53"/>
-      <c r="I78" s="53"/>
+      <c r="A78" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B78" s="51"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="51"/>
+      <c r="E78" s="51"/>
+      <c r="F78" s="51"/>
+      <c r="G78" s="51"/>
+      <c r="H78" s="51"/>
+      <c r="I78" s="51"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="53"/>
-      <c r="B79" s="53"/>
-      <c r="C79" s="53"/>
-      <c r="D79" s="53"/>
-      <c r="E79" s="53"/>
-      <c r="F79" s="53"/>
-      <c r="G79" s="53"/>
-      <c r="H79" s="53"/>
-      <c r="I79" s="53"/>
+      <c r="A79" s="51"/>
+      <c r="B79" s="51"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="51"/>
+      <c r="E79" s="51"/>
+      <c r="F79" s="51"/>
+      <c r="G79" s="51"/>
+      <c r="H79" s="51"/>
+      <c r="I79" s="51"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="21"/>
@@ -2059,17 +2059,17 @@
       <c r="I80" s="21"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="B81" s="54"/>
-      <c r="C81" s="54"/>
-      <c r="D81" s="54"/>
-      <c r="E81" s="54"/>
-      <c r="F81" s="54"/>
-      <c r="G81" s="54"/>
-      <c r="H81" s="54"/>
-      <c r="I81" s="54"/>
+      <c r="A81" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="B81" s="64"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="64"/>
+      <c r="H81" s="64"/>
+      <c r="I81" s="64"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
@@ -2083,28 +2083,28 @@
       <c r="I82" s="10"/>
     </row>
     <row r="83" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="B83" s="53"/>
-      <c r="C83" s="53"/>
-      <c r="D83" s="53"/>
-      <c r="E83" s="53"/>
-      <c r="F83" s="53"/>
-      <c r="G83" s="53"/>
-      <c r="H83" s="53"/>
-      <c r="I83" s="53"/>
+      <c r="A83" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B83" s="51"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="51"/>
+      <c r="E83" s="51"/>
+      <c r="F83" s="51"/>
+      <c r="G83" s="51"/>
+      <c r="H83" s="51"/>
+      <c r="I83" s="51"/>
     </row>
     <row r="84" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="53"/>
-      <c r="B84" s="53"/>
-      <c r="C84" s="53"/>
-      <c r="D84" s="53"/>
-      <c r="E84" s="53"/>
-      <c r="F84" s="53"/>
-      <c r="G84" s="53"/>
-      <c r="H84" s="53"/>
-      <c r="I84" s="53"/>
+      <c r="A84" s="51"/>
+      <c r="B84" s="51"/>
+      <c r="C84" s="51"/>
+      <c r="D84" s="51"/>
+      <c r="E84" s="51"/>
+      <c r="F84" s="51"/>
+      <c r="G84" s="51"/>
+      <c r="H84" s="51"/>
+      <c r="I84" s="51"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="86" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B86" s="52"/>
       <c r="C86" s="52"/>
@@ -2142,25 +2142,25 @@
       <c r="I87" s="10"/>
     </row>
     <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="46" t="s">
+      <c r="A88" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" s="40"/>
+      <c r="C88" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B88" s="46"/>
-      <c r="C88" s="47" t="s">
+      <c r="D88" s="41"/>
+      <c r="E88" s="41"/>
+      <c r="F88" s="41"/>
+      <c r="G88" s="41"/>
+      <c r="H88" s="41"/>
+      <c r="I88" s="41"/>
+    </row>
+    <row r="89" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="40"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="52" t="s">
         <v>67</v>
-      </c>
-      <c r="D88" s="47"/>
-      <c r="E88" s="47"/>
-      <c r="F88" s="47"/>
-      <c r="G88" s="47"/>
-      <c r="H88" s="47"/>
-      <c r="I88" s="47"/>
-    </row>
-    <row r="89" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="46"/>
-      <c r="B89" s="46"/>
-      <c r="C89" s="52" t="s">
-        <v>68</v>
       </c>
       <c r="D89" s="52"/>
       <c r="E89" s="52"/>
@@ -2181,28 +2181,28 @@
       <c r="I90" s="10"/>
     </row>
     <row r="91" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B91" s="53"/>
-      <c r="C91" s="53"/>
-      <c r="D91" s="53"/>
-      <c r="E91" s="53"/>
-      <c r="F91" s="53"/>
-      <c r="G91" s="53"/>
-      <c r="H91" s="53"/>
-      <c r="I91" s="53"/>
+      <c r="A91" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B91" s="51"/>
+      <c r="C91" s="51"/>
+      <c r="D91" s="51"/>
+      <c r="E91" s="51"/>
+      <c r="F91" s="51"/>
+      <c r="G91" s="51"/>
+      <c r="H91" s="51"/>
+      <c r="I91" s="51"/>
     </row>
     <row r="92" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="53"/>
-      <c r="B92" s="53"/>
-      <c r="C92" s="53"/>
-      <c r="D92" s="53"/>
-      <c r="E92" s="53"/>
-      <c r="F92" s="53"/>
-      <c r="G92" s="53"/>
-      <c r="H92" s="53"/>
-      <c r="I92" s="53"/>
+      <c r="A92" s="51"/>
+      <c r="B92" s="51"/>
+      <c r="C92" s="51"/>
+      <c r="D92" s="51"/>
+      <c r="E92" s="51"/>
+      <c r="F92" s="51"/>
+      <c r="G92" s="51"/>
+      <c r="H92" s="51"/>
+      <c r="I92" s="51"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
@@ -2216,10 +2216,10 @@
       <c r="I93" s="10"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B94" s="51"/>
+      <c r="A94" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B94" s="63"/>
       <c r="C94" s="20"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -2232,14 +2232,14 @@
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="19"/>
-      <c r="D95" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="E95" s="69"/>
-      <c r="F95" s="69"/>
-      <c r="G95" s="69"/>
-      <c r="H95" s="69"/>
-      <c r="I95" s="69"/>
+      <c r="D95" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E95" s="43"/>
+      <c r="F95" s="43"/>
+      <c r="G95" s="43"/>
+      <c r="H95" s="43"/>
+      <c r="I95" s="43"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
@@ -2253,11 +2253,11 @@
       <c r="I96" s="10"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B97" s="51"/>
-      <c r="C97" s="51"/>
+      <c r="A97" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B97" s="63"/>
+      <c r="C97" s="63"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
@@ -2269,14 +2269,14 @@
       <c r="A98" s="10"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
-      <c r="D98" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="E98" s="69"/>
-      <c r="F98" s="69"/>
-      <c r="G98" s="69"/>
-      <c r="H98" s="69"/>
-      <c r="I98" s="69"/>
+      <c r="D98" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E98" s="43"/>
+      <c r="F98" s="43"/>
+      <c r="G98" s="43"/>
+      <c r="H98" s="43"/>
+      <c r="I98" s="43"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
@@ -2304,53 +2304,53 @@
       <c r="A101" s="10"/>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
-      <c r="D101" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="E101" s="70"/>
-      <c r="F101" s="70"/>
+      <c r="D101" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E101" s="45"/>
+      <c r="F101" s="45"/>
       <c r="G101" s="10"/>
       <c r="H101" s="10"/>
       <c r="I101" s="10"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="67" t="s">
+      <c r="A102" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B102" s="56"/>
+      <c r="C102" s="56"/>
+      <c r="D102" s="56"/>
+      <c r="E102" s="56"/>
+      <c r="F102" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="B102" s="68"/>
-      <c r="C102" s="68"/>
-      <c r="D102" s="68"/>
-      <c r="E102" s="68"/>
-      <c r="F102" s="67" t="s">
+      <c r="G102" s="55"/>
+      <c r="H102" s="55"/>
+      <c r="I102" s="55"/>
+    </row>
+    <row r="103" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="G102" s="67"/>
-      <c r="H102" s="67"/>
-      <c r="I102" s="67"/>
-    </row>
-    <row r="103" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="65" t="s">
+      <c r="B103" s="53"/>
+      <c r="C103" s="53"/>
+      <c r="D103" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B103" s="65"/>
-      <c r="C103" s="65"/>
-      <c r="D103" s="14" t="s">
+      <c r="E103" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="E103" s="14" t="s">
+      <c r="F103" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F103" s="14" t="s">
-        <v>79</v>
-      </c>
       <c r="G103" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H103" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I103" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="H103" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I103" s="14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -2378,33 +2378,33 @@
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="10"/>
-      <c r="C106" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="D106" s="64"/>
-      <c r="E106" s="64"/>
-      <c r="F106" s="64"/>
-      <c r="G106" s="64"/>
+      <c r="C106" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D106" s="44"/>
+      <c r="E106" s="44"/>
+      <c r="F106" s="44"/>
+      <c r="G106" s="44"/>
       <c r="H106" s="10"/>
       <c r="I106" s="10"/>
     </row>
     <row r="107" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="65" t="s">
+      <c r="A107" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B107" s="54"/>
+      <c r="C107" s="54"/>
+      <c r="D107" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B107" s="66"/>
-      <c r="C107" s="66"/>
-      <c r="D107" s="65" t="s">
-        <v>82</v>
-      </c>
-      <c r="E107" s="66"/>
-      <c r="F107" s="66"/>
-      <c r="G107" s="65" t="s">
+      <c r="E107" s="54"/>
+      <c r="F107" s="54"/>
+      <c r="G107" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="H107" s="53"/>
+      <c r="I107" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="H107" s="65"/>
-      <c r="I107" s="14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -2420,20 +2420,71 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="A62:I62"/>
-    <mergeCell ref="A69:B70"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="C66:I66"/>
-    <mergeCell ref="C69:I69"/>
-    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="A50:I50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A13:B14"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="A97:C97"/>
+    <mergeCell ref="A66:B67"/>
+    <mergeCell ref="C67:I67"/>
+    <mergeCell ref="A78:I79"/>
+    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A91:I92"/>
+    <mergeCell ref="C76:I76"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="A107:C107"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="A103:C103"/>
     <mergeCell ref="D98:I98"/>
     <mergeCell ref="D101:F101"/>
     <mergeCell ref="D95:I95"/>
@@ -2450,71 +2501,20 @@
     <mergeCell ref="C75:I75"/>
     <mergeCell ref="C88:I88"/>
     <mergeCell ref="C73:I73"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="A107:C107"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="G107:H107"/>
-    <mergeCell ref="A102:E102"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="A103:C103"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="A97:C97"/>
-    <mergeCell ref="A66:B67"/>
-    <mergeCell ref="C67:I67"/>
-    <mergeCell ref="A78:I79"/>
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A91:I92"/>
-    <mergeCell ref="C76:I76"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A13:B14"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A50:I50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A69:B70"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="C66:I66"/>
+    <mergeCell ref="C69:I69"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="A58:I58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>